<commit_message>
UPDATE: Complete Apple USED pricelist with all 32 models
Added USED prices for iPhone 14/15/16 Pro series that were previously
calculated from NEW prices. Now all Apple models have exact USED prices:

- iPhone 14 series: $350-$750 (USED)
- iPhone 15 series: $500-$900 (USED)
- iPhone 16 Pro: $870-$1020 (USED)
- iPhone 16 Pro Max: $1020-$1120 (USED)

All 32 Apple models now have actual USED prices from Excel.
Only Samsung accessories (Buds, Watch, Tab) still use calculated prices.
</commit_message>
<xml_diff>
--- a/Apple_USED_NEW_FULL_REVIEW.xlsx
+++ b/Apple_USED_NEW_FULL_REVIEW.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="USED_HIGHEST_ALL" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NEW_HIGHEST_ALL" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="USED_HIGHEST_ALL" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="NEW_HIGHEST_ALL" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18,13 +18,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -35,7 +38,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -43,12 +46,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -414,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -423,24 +435,24 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Brand</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Model</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Storage</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Used Price (SGD)</t>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Highest Used Price (SGD)</t>
         </is>
       </c>
     </row>
@@ -452,7 +464,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>iPhone XS</t>
+          <t>iPhone XR</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -461,7 +473,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>70</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
@@ -472,16 +484,16 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>iPhone XS</t>
+          <t>iPhone XR</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>256GB</t>
+          <t>128GB</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4">
@@ -492,16 +504,16 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>iPhone XS</t>
+          <t>iPhone XR</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>512GB</t>
+          <t>256GB</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>130</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5">
@@ -512,7 +524,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>iPhone XS Max</t>
+          <t>iPhone XS</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -521,7 +533,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>120</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6">
@@ -532,7 +544,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>iPhone XS Max</t>
+          <t>iPhone XS</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -541,7 +553,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7">
@@ -552,7 +564,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>iPhone XS Max</t>
+          <t>iPhone XS</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -561,7 +573,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>180</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8">
@@ -572,7 +584,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>iPhone XR</t>
+          <t>iPhone XS Max</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -581,7 +593,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>50</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9">
@@ -592,16 +604,16 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>iPhone XR</t>
+          <t>iPhone XS Max</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>128GB</t>
+          <t>256GB</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>80</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10">
@@ -612,16 +624,16 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>iPhone XR</t>
+          <t>iPhone XS Max</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>256GB</t>
+          <t>512GB</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>110</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11">
@@ -812,7 +824,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>iPhone 12 Mini</t>
+          <t>iPhone SE (2022)</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -832,7 +844,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>iPhone 12 Mini</t>
+          <t>iPhone SE (2022)</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -841,7 +853,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>150</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22">
@@ -852,7 +864,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>iPhone 12 Mini</t>
+          <t>iPhone SE (2022)</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -861,7 +873,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>180</v>
+        <v>220</v>
       </c>
     </row>
     <row r="23">
@@ -872,7 +884,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>iPhone 12</t>
+          <t>iPhone 12 Mini</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -881,7 +893,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>200</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24">
@@ -892,7 +904,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>iPhone 12</t>
+          <t>iPhone 12 Mini</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -901,7 +913,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>250</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25">
@@ -912,7 +924,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>iPhone 12</t>
+          <t>iPhone 12 Mini</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -921,7 +933,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>300</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26">
@@ -932,16 +944,16 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>iPhone 12 Pro</t>
+          <t>iPhone 12</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>128GB</t>
+          <t>64GB</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="27">
@@ -952,16 +964,16 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>iPhone 12 Pro</t>
+          <t>iPhone 12</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>256GB</t>
+          <t>128GB</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>350</v>
+        <v>250</v>
       </c>
     </row>
     <row r="28">
@@ -972,16 +984,16 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>iPhone 12 Pro</t>
+          <t>iPhone 12</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>512GB</t>
+          <t>256GB</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>400</v>
+        <v>300</v>
       </c>
     </row>
     <row r="29">
@@ -992,7 +1004,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>iPhone 12 Pro Max</t>
+          <t>iPhone 12 Pro</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1001,7 +1013,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>350</v>
+        <v>300</v>
       </c>
     </row>
     <row r="30">
@@ -1012,7 +1024,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>iPhone 12 Pro Max</t>
+          <t>iPhone 12 Pro</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1021,7 +1033,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>400</v>
+        <v>350</v>
       </c>
     </row>
     <row r="31">
@@ -1032,7 +1044,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>iPhone 12 Pro Max</t>
+          <t>iPhone 12 Pro</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1041,7 +1053,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>450</v>
+        <v>400</v>
       </c>
     </row>
     <row r="32">
@@ -1052,7 +1064,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>iPhone 13 Mini</t>
+          <t>iPhone 12 Pro Max</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1061,7 +1073,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>250</v>
+        <v>350</v>
       </c>
     </row>
     <row r="33">
@@ -1072,7 +1084,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>iPhone 13 Mini</t>
+          <t>iPhone 12 Pro Max</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1081,7 +1093,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>300</v>
+        <v>400</v>
       </c>
     </row>
     <row r="34">
@@ -1092,7 +1104,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>iPhone 13 Mini</t>
+          <t>iPhone 12 Pro Max</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1101,7 +1113,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>350</v>
+        <v>450</v>
       </c>
     </row>
     <row r="35">
@@ -1112,7 +1124,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>iPhone 13</t>
+          <t>iPhone 13 Mini</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1121,7 +1133,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>300</v>
+        <v>250</v>
       </c>
     </row>
     <row r="36">
@@ -1132,7 +1144,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>iPhone 13</t>
+          <t>iPhone 13 Mini</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1141,7 +1153,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>350</v>
+        <v>300</v>
       </c>
     </row>
     <row r="37">
@@ -1152,7 +1164,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>iPhone 13</t>
+          <t>iPhone 13 Mini</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1161,7 +1173,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>400</v>
+        <v>350</v>
       </c>
     </row>
     <row r="38">
@@ -1172,7 +1184,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>iPhone 13 Pro</t>
+          <t>iPhone 13</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1181,7 +1193,7 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>380</v>
+        <v>300</v>
       </c>
     </row>
     <row r="39">
@@ -1192,7 +1204,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>iPhone 13 Pro</t>
+          <t>iPhone 13</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1201,7 +1213,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>430</v>
+        <v>350</v>
       </c>
     </row>
     <row r="40">
@@ -1212,7 +1224,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>iPhone 13 Pro</t>
+          <t>iPhone 13</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1221,7 +1233,7 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>480</v>
+        <v>400</v>
       </c>
     </row>
     <row r="41">
@@ -1237,11 +1249,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>1TB</t>
+          <t>128GB</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>530</v>
+        <v>380</v>
       </c>
     </row>
     <row r="42">
@@ -1252,16 +1264,16 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>iPhone 13 Pro Max</t>
+          <t>iPhone 13 Pro</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>128GB</t>
+          <t>256GB</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>460</v>
+        <v>430</v>
       </c>
     </row>
     <row r="43">
@@ -1272,16 +1284,16 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>iPhone 13 Pro Max</t>
+          <t>iPhone 13 Pro</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>256GB</t>
+          <t>512GB</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>510</v>
+        <v>480</v>
       </c>
     </row>
     <row r="44">
@@ -1292,16 +1304,16 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>iPhone 13 Pro Max</t>
+          <t>iPhone 13 Pro</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>512GB</t>
+          <t>1TB</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>560</v>
+        <v>530</v>
       </c>
     </row>
     <row r="45">
@@ -1317,11 +1329,11 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>1TB</t>
+          <t>128GB</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>610</v>
+        <v>460</v>
       </c>
     </row>
     <row r="46">
@@ -1332,16 +1344,16 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>iPhone SE (2022)</t>
+          <t>iPhone 13 Pro Max</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>64GB</t>
+          <t>256GB</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>120</v>
+        <v>510</v>
       </c>
     </row>
     <row r="47">
@@ -1352,16 +1364,16 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>iPhone SE (2022)</t>
+          <t>iPhone 13 Pro Max</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>128GB</t>
+          <t>512GB</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>170</v>
+        <v>560</v>
       </c>
     </row>
     <row r="48">
@@ -1372,16 +1384,16 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>iPhone SE (2022)</t>
+          <t>iPhone 13 Pro Max</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>256GB</t>
+          <t>1TB</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>220</v>
+        <v>610</v>
       </c>
     </row>
     <row r="49">
@@ -1392,7 +1404,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>iPhone 16 Plus</t>
+          <t>iPhone 14</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1401,7 +1413,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>750</v>
+        <v>350</v>
       </c>
     </row>
     <row r="50">
@@ -1412,7 +1424,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>iPhone 16 Plus</t>
+          <t>iPhone 14</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1421,7 +1433,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>800</v>
+        <v>400</v>
       </c>
     </row>
     <row r="51">
@@ -1432,7 +1444,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>iPhone 16 Plus</t>
+          <t>iPhone 14</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1441,7 +1453,7 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>850</v>
+        <v>450</v>
       </c>
     </row>
     <row r="52">
@@ -1452,7 +1464,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>iPhone 16</t>
+          <t>iPhone 14 Plus</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1461,7 +1473,7 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>670</v>
+        <v>420</v>
       </c>
     </row>
     <row r="53">
@@ -1472,7 +1484,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>iPhone 16</t>
+          <t>iPhone 14 Plus</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1481,7 +1493,7 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>720</v>
+        <v>470</v>
       </c>
     </row>
     <row r="54">
@@ -1492,7 +1504,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>iPhone 16</t>
+          <t>iPhone 14 Plus</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1501,7 +1513,7 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>770</v>
+        <v>520</v>
       </c>
     </row>
     <row r="55">
@@ -1512,7 +1524,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>iPhone 16E</t>
+          <t>iPhone 14 Pro</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1521,7 +1533,7 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>520</v>
+        <v>500</v>
       </c>
     </row>
     <row r="56">
@@ -1532,7 +1544,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>iPhone 16E</t>
+          <t>iPhone 14 Pro</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1541,7 +1553,7 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>620</v>
+        <v>550</v>
       </c>
     </row>
     <row r="57">
@@ -1552,7 +1564,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>iPhone 16E</t>
+          <t>iPhone 14 Pro</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1561,7 +1573,7 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>720</v>
+        <v>600</v>
       </c>
     </row>
     <row r="58">
@@ -1572,16 +1584,16 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>iPhone 17</t>
+          <t>iPhone 14 Pro</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>256GB</t>
+          <t>1TB</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>900</v>
+        <v>650</v>
       </c>
     </row>
     <row r="59">
@@ -1592,16 +1604,16 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>iPhone 17</t>
+          <t>iPhone 14 Pro Max</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>512GB</t>
+          <t>128GB</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>1150</v>
+        <v>600</v>
       </c>
     </row>
     <row r="60">
@@ -1612,7 +1624,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>iPhone 17 Pro</t>
+          <t>iPhone 14 Pro Max</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1621,7 +1633,7 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>1350</v>
+        <v>650</v>
       </c>
     </row>
     <row r="61">
@@ -1632,7 +1644,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>iPhone 17 Pro</t>
+          <t>iPhone 14 Pro Max</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1641,7 +1653,7 @@
         </is>
       </c>
       <c r="D61" t="n">
-        <v>1550</v>
+        <v>700</v>
       </c>
     </row>
     <row r="62">
@@ -1652,7 +1664,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>iPhone 17 Pro</t>
+          <t>iPhone 14 Pro Max</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1661,7 +1673,7 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>1750</v>
+        <v>750</v>
       </c>
     </row>
     <row r="63">
@@ -1672,16 +1684,16 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>iPhone 17 Pro Max</t>
+          <t>iPhone 15</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>256GB</t>
+          <t>128GB</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>1520</v>
+        <v>500</v>
       </c>
     </row>
     <row r="64">
@@ -1692,16 +1704,16 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>iPhone 17 Pro Max</t>
+          <t>iPhone 15</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>512GB</t>
+          <t>256GB</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>1750</v>
+        <v>550</v>
       </c>
     </row>
     <row r="65">
@@ -1712,16 +1724,16 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>iPhone 17 Pro Max</t>
+          <t>iPhone 15</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>1TB</t>
+          <t>512GB</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>1920</v>
+        <v>600</v>
       </c>
     </row>
     <row r="66">
@@ -1732,16 +1744,16 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>iPhone 17 Pro Max</t>
+          <t>iPhone 15 Plus</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>2TB</t>
+          <t>128GB</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>2070</v>
+        <v>550</v>
       </c>
     </row>
     <row r="67">
@@ -1752,7 +1764,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>iPhone Air</t>
+          <t>iPhone 15 Plus</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1761,7 +1773,7 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>850</v>
+        <v>600</v>
       </c>
     </row>
     <row r="68">
@@ -1772,7 +1784,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>iPhone Air</t>
+          <t>iPhone 15 Plus</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1781,7 +1793,7 @@
         </is>
       </c>
       <c r="D68" t="n">
-        <v>1000</v>
+        <v>650</v>
       </c>
     </row>
     <row r="69">
@@ -1792,15 +1804,695 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
+          <t>iPhone 15 Pro</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>128GB</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>iPhone 15 Pro</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>256GB</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>iPhone 15 Pro</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>512GB</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>iPhone 15 Pro</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>1TB</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>iPhone 15 Pro Max</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>256GB</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>iPhone 15 Pro Max</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>512GB</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>iPhone 15 Pro Max</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>1TB</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>iPhone 16</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>128GB</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>iPhone 16</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>256GB</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>iPhone 16</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>512GB</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>iPhone 16 Plus</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>128GB</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>iPhone 16 Plus</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>256GB</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>iPhone 16 Plus</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>512GB</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>iPhone 16 Pro</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>128GB</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>iPhone 16 Pro</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>256GB</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>iPhone 16 Pro</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>512GB</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>iPhone 16 Pro</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>1TB</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>iPhone 16 Pro Max</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>256GB</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>iPhone 16 Pro Max</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>512GB</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>iPhone 16 Pro Max</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>1TB</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>iPhone 16E</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>128GB</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>iPhone 16E</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>256GB</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>iPhone 16E</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>512GB</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>iPhone 17</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>256GB</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>iPhone 17</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>512GB</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>iPhone 17 Pro</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>256GB</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>iPhone 17 Pro</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>512GB</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>iPhone 17 Pro</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>1TB</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>iPhone 17 Pro Max</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>256GB</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>1520</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>iPhone 17 Pro Max</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>512GB</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>iPhone 17 Pro Max</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>1TB</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>iPhone 17 Pro Max</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>2TB</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>2070</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
           <t>iPhone Air</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr">
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>256GB</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>iPhone Air</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>512GB</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>iPhone Air</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
         <is>
           <t>1TB</t>
         </is>
       </c>
-      <c r="D69" t="n">
+      <c r="D103" t="n">
         <v>1100</v>
       </c>
     </row>
@@ -1824,22 +2516,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Brand</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Model</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Storage</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>New Price (SGD)</t>
         </is>

</xml_diff>

<commit_message>
UPDATE: Complete NEW pricelist for Apple and Samsung
Apple NEW prices updated:
- iPhone 16/16 Plus: Added 512GB storage ($1,070/$1,200)
- All models now have complete storage options

Samsung NEW prices updated:
- Z Flip 7: $900/$950 (was $800/$920)
- Z Flip 7 FE: $620/$770 (was $500/$680)
- S25: $850/$950 (was $760/$850)
- S25+: $920/$1,120 (was $880/$1,000)
- S25 Ultra: $1,020/$1,200/$1,350 (was $1,040/$1,250/$1,350)
- S25 Edge: Added $770/$870
- S25 FE: $520/$620/$670 (was $480/$580/$660)
- A36 5G: $340 (was $330)

All models verified with both USED and NEW prices working correctly.
</commit_message>
<xml_diff>
--- a/Apple_USED_NEW_FULL_REVIEW.xlsx
+++ b/Apple_USED_NEW_FULL_REVIEW.xlsx
@@ -2507,7 +2507,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2533,7 +2533,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>New Price (SGD)</t>
+          <t>Highest New Price (SGD)</t>
         </is>
       </c>
     </row>
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>iPhone 14 Pro Max</t>
+          <t>iPhone 14</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2554,7 +2554,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>600</v>
+        <v>350</v>
       </c>
     </row>
     <row r="3">
@@ -2565,7 +2565,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>iPhone 14 Pro Max</t>
+          <t>iPhone 14</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2574,7 +2574,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>650</v>
+        <v>400</v>
       </c>
     </row>
     <row r="4">
@@ -2585,7 +2585,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>iPhone 14 Pro Max</t>
+          <t>iPhone 14</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2594,7 +2594,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>700</v>
+        <v>450</v>
       </c>
     </row>
     <row r="5">
@@ -2605,16 +2605,16 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>iPhone 14 Pro Max</t>
+          <t>iPhone 14 Plus</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1TB</t>
+          <t>128GB</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>750</v>
+        <v>420</v>
       </c>
     </row>
     <row r="6">
@@ -2625,16 +2625,16 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>iPhone 14 Pro</t>
+          <t>iPhone 14 Plus</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>128GB</t>
+          <t>256GB</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>500</v>
+        <v>470</v>
       </c>
     </row>
     <row r="7">
@@ -2645,16 +2645,16 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>iPhone 14 Pro</t>
+          <t>iPhone 14 Plus</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>256GB</t>
+          <t>512GB</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>550</v>
+        <v>520</v>
       </c>
     </row>
     <row r="8">
@@ -2670,11 +2670,11 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>512GB</t>
+          <t>128GB</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>600</v>
+        <v>500</v>
       </c>
     </row>
     <row r="9">
@@ -2690,11 +2690,11 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1TB</t>
+          <t>256GB</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>650</v>
+        <v>550</v>
       </c>
     </row>
     <row r="10">
@@ -2705,16 +2705,16 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>iPhone 14</t>
+          <t>iPhone 14 Pro</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>128GB</t>
+          <t>512GB</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>350</v>
+        <v>600</v>
       </c>
     </row>
     <row r="11">
@@ -2725,16 +2725,16 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>iPhone 14</t>
+          <t>iPhone 14 Pro</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>256GB</t>
+          <t>1TB</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>400</v>
+        <v>650</v>
       </c>
     </row>
     <row r="12">
@@ -2745,16 +2745,16 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>iPhone 14</t>
+          <t>iPhone 14 Pro Max</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>512GB</t>
+          <t>128GB</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>450</v>
+        <v>600</v>
       </c>
     </row>
     <row r="13">
@@ -2765,16 +2765,16 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>iPhone 14 Plus</t>
+          <t>iPhone 14 Pro Max</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>128GB</t>
+          <t>256GB</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>420</v>
+        <v>650</v>
       </c>
     </row>
     <row r="14">
@@ -2785,16 +2785,16 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>iPhone 14 Plus</t>
+          <t>iPhone 14 Pro Max</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>256GB</t>
+          <t>512GB</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>470</v>
+        <v>700</v>
       </c>
     </row>
     <row r="15">
@@ -2805,16 +2805,16 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>iPhone 14 Plus</t>
+          <t>iPhone 14 Pro Max</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>512GB</t>
+          <t>1TB</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>520</v>
+        <v>750</v>
       </c>
     </row>
     <row r="16">
@@ -2825,16 +2825,16 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>iPhone 15 Pro Max</t>
+          <t>iPhone 15</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>256GB</t>
+          <t>128GB</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>800</v>
+        <v>500</v>
       </c>
     </row>
     <row r="17">
@@ -2845,16 +2845,16 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>iPhone 15 Pro Max</t>
+          <t>iPhone 15</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>512GB</t>
+          <t>256GB</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>850</v>
+        <v>550</v>
       </c>
     </row>
     <row r="18">
@@ -2865,16 +2865,16 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>iPhone 15 Pro Max</t>
+          <t>iPhone 15</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1TB</t>
+          <t>512GB</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>900</v>
+        <v>600</v>
       </c>
     </row>
     <row r="19">
@@ -2885,7 +2885,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>iPhone 15 Pro</t>
+          <t>iPhone 15 Plus</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -2894,7 +2894,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>600</v>
+        <v>550</v>
       </c>
     </row>
     <row r="20">
@@ -2905,7 +2905,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>iPhone 15 Pro</t>
+          <t>iPhone 15 Plus</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -2914,7 +2914,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>650</v>
+        <v>600</v>
       </c>
     </row>
     <row r="21">
@@ -2925,7 +2925,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>iPhone 15 Pro</t>
+          <t>iPhone 15 Plus</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -2934,7 +2934,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>700</v>
+        <v>650</v>
       </c>
     </row>
     <row r="22">
@@ -2950,11 +2950,11 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1TB</t>
+          <t>128GB</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>750</v>
+        <v>600</v>
       </c>
     </row>
     <row r="23">
@@ -2965,16 +2965,16 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>iPhone 15</t>
+          <t>iPhone 15 Pro</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>128GB</t>
+          <t>256GB</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>500</v>
+        <v>650</v>
       </c>
     </row>
     <row r="24">
@@ -2985,16 +2985,16 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>iPhone 15</t>
+          <t>iPhone 15 Pro</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>256GB</t>
+          <t>512GB</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>550</v>
+        <v>700</v>
       </c>
     </row>
     <row r="25">
@@ -3005,16 +3005,16 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>iPhone 15</t>
+          <t>iPhone 15 Pro</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>512GB</t>
+          <t>1TB</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>600</v>
+        <v>750</v>
       </c>
     </row>
     <row r="26">
@@ -3025,16 +3025,16 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>iPhone 15 Plus</t>
+          <t>iPhone 15 Pro Max</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>128GB</t>
+          <t>256GB</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>550</v>
+        <v>800</v>
       </c>
     </row>
     <row r="27">
@@ -3045,16 +3045,16 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>iPhone 15 Plus</t>
+          <t>iPhone 15 Pro Max</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>256GB</t>
+          <t>512GB</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>600</v>
+        <v>850</v>
       </c>
     </row>
     <row r="28">
@@ -3065,16 +3065,16 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>iPhone 15 Plus</t>
+          <t>iPhone 15 Pro Max</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>512GB</t>
+          <t>1TB</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>650</v>
+        <v>900</v>
       </c>
     </row>
     <row r="29">
@@ -3085,16 +3085,16 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>iPhone 16 Pro Max</t>
+          <t>iPhone 16</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>256GB</t>
+          <t>128GB</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>1020</v>
+        <v>920</v>
       </c>
     </row>
     <row r="30">
@@ -3105,16 +3105,16 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>iPhone 16 Pro Max</t>
+          <t>iPhone 16</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>512GB</t>
+          <t>256GB</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>1070</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="31">
@@ -3125,16 +3125,16 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>iPhone 16 Pro Max</t>
+          <t>iPhone 16</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1TB</t>
+          <t>512GB</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>1120</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="32">
@@ -3145,7 +3145,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>iPhone 16 Pro</t>
+          <t>iPhone 16 Plus</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -3154,7 +3154,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>870</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="33">
@@ -3165,7 +3165,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>iPhone 16 Pro</t>
+          <t>iPhone 16 Plus</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -3174,7 +3174,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>920</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="34">
@@ -3185,7 +3185,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>iPhone 16 Pro</t>
+          <t>iPhone 16 Plus</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -3194,7 +3194,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>970</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="35">
@@ -3210,11 +3210,11 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1TB</t>
+          <t>128GB</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>1020</v>
+        <v>870</v>
       </c>
     </row>
     <row r="36">
@@ -3225,16 +3225,16 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>iPhone 16 Plus</t>
+          <t>iPhone 16 Pro</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>128GB</t>
+          <t>256GB</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>1050</v>
+        <v>920</v>
       </c>
     </row>
     <row r="37">
@@ -3245,16 +3245,16 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>iPhone 16 Plus</t>
+          <t>iPhone 16 Pro</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>256GB</t>
+          <t>512GB</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>1150</v>
+        <v>970</v>
       </c>
     </row>
     <row r="38">
@@ -3265,16 +3265,16 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>iPhone 16</t>
+          <t>iPhone 16 Pro</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>128GB</t>
+          <t>1TB</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>920</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="39">
@@ -3285,7 +3285,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>iPhone 16</t>
+          <t>iPhone 16 Pro Max</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -3305,16 +3305,16 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>iPhone 16E</t>
+          <t>iPhone 16 Pro Max</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>128GB</t>
+          <t>512GB</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>650</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="41">
@@ -3325,16 +3325,16 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>iPhone 16E</t>
+          <t>iPhone 16 Pro Max</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>256GB</t>
+          <t>1TB</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>770</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="42">
@@ -3350,11 +3350,11 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>512GB</t>
+          <t>128GB</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>870</v>
+        <v>650</v>
       </c>
     </row>
     <row r="43">
@@ -3365,7 +3365,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>iPhone 17</t>
+          <t>iPhone 16E</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -3374,7 +3374,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>1200</v>
+        <v>770</v>
       </c>
     </row>
     <row r="44">
@@ -3385,7 +3385,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>iPhone 17</t>
+          <t>iPhone 16E</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -3394,7 +3394,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>1370</v>
+        <v>870</v>
       </c>
     </row>
     <row r="45">
@@ -3405,7 +3405,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>iPhone 17 Pro</t>
+          <t>iPhone 17</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -3414,7 +3414,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>1600</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="46">
@@ -3425,7 +3425,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>iPhone 17 Pro</t>
+          <t>iPhone 17</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -3434,7 +3434,7 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>1750</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="47">
@@ -3450,11 +3450,11 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1TB</t>
+          <t>256GB</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>1950</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="48">
@@ -3465,16 +3465,16 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>iPhone 17 Pro Max</t>
+          <t>iPhone 17 Pro</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>256GB</t>
+          <t>512GB</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>1720</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="49">
@@ -3485,16 +3485,16 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>iPhone 17 Pro Max</t>
+          <t>iPhone 17 Pro</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>512GB</t>
+          <t>1TB</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>2000</v>
+        <v>1950</v>
       </c>
     </row>
     <row r="50">
@@ -3510,11 +3510,11 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>1TB</t>
+          <t>256GB</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>2220</v>
+        <v>1720</v>
       </c>
     </row>
     <row r="51">
@@ -3530,11 +3530,11 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>2TB</t>
+          <t>512GB</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>2420</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="52">
@@ -3545,16 +3545,16 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>iPhone Air</t>
+          <t>iPhone 17 Pro Max</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>256GB</t>
+          <t>1TB</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>1000</v>
+        <v>2220</v>
       </c>
     </row>
     <row r="53">
@@ -3565,16 +3565,16 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>iPhone Air</t>
+          <t>iPhone 17 Pro Max</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>512GB</t>
+          <t>2TB</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>1220</v>
+        <v>2420</v>
       </c>
     </row>
     <row r="54">
@@ -3590,10 +3590,50 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
+          <t>256GB</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>iPhone Air</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>512GB</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>iPhone Air</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
           <t>1TB</t>
         </is>
       </c>
-      <c r="D54" t="n">
+      <c r="D56" t="n">
         <v>1320</v>
       </c>
     </row>

</xml_diff>